<commit_message>
Should have made it so Protocols have MKB Izpylnitel i DZH izpylnitel
</commit_message>
<xml_diff>
--- a/Files/50000-51000/50278/50278_RequestList.xlsx
+++ b/Files/50000-51000/50278/50278_RequestList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ФК 404-4</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>Млечно изследване 2</t>
+  </si>
+  <si>
+    <t>marto</t>
+  </si>
+  <si>
+    <t>Киселинност</t>
+  </si>
+  <si>
+    <t>Бацилус</t>
+  </si>
+  <si>
+    <t>Ешерихия коли</t>
   </si>
   <si>
     <t>Срок за изпитване: 3 дни</t>
@@ -472,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:F5"/>
@@ -552,34 +564,66 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="10">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" ht="18.75">
-      <c r="A11" s="8"/>
-      <c r="B11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="3" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="11">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="12">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="8"/>
+    </row>
+    <row r="15" ht="18.75">
+      <c r="A15" s="8"/>
+      <c r="B15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="8"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Working on Queries File
</commit_message>
<xml_diff>
--- a/Files/50000-51000/50278/50278_RequestList.xlsx
+++ b/Files/50000-51000/50278/50278_RequestList.xlsx
@@ -14,62 +14,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>ФК 404-4</t>
-  </si>
-  <si>
-    <t>ЛАБОРАТОРИЯ ЗА ИЗПИТВАНЕ КЪМ РВС – РУСЕ ЕООД</t>
-  </si>
-  <si>
-    <t>ЗАЯВКА № 50278 / Дата 13.11.2015 г / Час 14:01</t>
-  </si>
-  <si>
-    <t>№</t>
-  </si>
-  <si>
-    <t>Вид на пробата</t>
-  </si>
-  <si>
-    <t>Брой/ количество</t>
-  </si>
-  <si>
-    <t>Показатели за изпитване</t>
-  </si>
-  <si>
-    <t>domat</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Млечно изследване 2</t>
-  </si>
-  <si>
-    <t>marto</t>
-  </si>
-  <si>
-    <t>Киселинност</t>
-  </si>
-  <si>
-    <t>Бацилус</t>
-  </si>
-  <si>
-    <t>Ешерихия коли</t>
-  </si>
-  <si>
-    <t>Срок за изпитване: 3 дни</t>
-  </si>
-  <si>
-    <t>Приел пробата:………….</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">ФК 404-4   </t>
+  </si>
+  <si>
+    <t>ЛАБОРАТОРИЯ ЗА ИЗПИТВАНЕ КЪМ "РВС – РУСЕ" ЕООД</t>
+  </si>
+  <si>
+    <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
+  </si>
+  <si>
+    <t>ЗАЯВКА № #NUMBER / Дата #DATE</t>
+  </si>
+  <si>
+    <t>7.1 МИКРОБИОЛОГИЧНО ИЗПИТВАНЕ</t>
+  </si>
+  <si>
+    <t>Вх. №</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вид на  пробата</t>
+  </si>
+  <si>
+    <t>Показател</t>
+  </si>
+  <si>
+    <t>Метод</t>
+  </si>
+  <si>
+    <t>Допуск</t>
+  </si>
+  <si>
+    <t>Забележка</t>
+  </si>
+  <si>
+    <t>Срок за изпитване: #D дни</t>
+  </si>
+  <si>
+    <t>Приел пробата......</t>
+  </si>
+  <si>
+    <t>7.2 ФИЗИКОХИМИЧНО И ОРГАНОЛЕПТИЧНО ИЗПИТВАНЕ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,18 +78,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -113,41 +95,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000" tint="0"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000" tint="0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000" tint="0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000" tint="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -155,30 +107,19 @@
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="0">
-      <alignment horizontal="center"/>
+    <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,143 +428,203 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75">
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="3" ht="18.75">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" ht="18.75">
       <c r="A4" s="1"/>
-    </row>
-    <row r="5" ht="18.75">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-    </row>
-    <row r="7" ht="36.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" ht="18.75">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="B9" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E9" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="E11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="8"/>
-    </row>
-    <row r="15" ht="18.75">
-      <c r="A15" s="8"/>
-      <c r="B15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="16">
-      <c r="A16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="8"/>
+      <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
+      <c r="A18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Almost done with Requests
</commit_message>
<xml_diff>
--- a/Files/50000-51000/50278/50278_RequestList.xlsx
+++ b/Files/50000-51000/50278/50278_RequestList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">ФК 404-4   </t>
   </si>
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t>ЗАЯВКА № #NUMBER / Дата #DATE</t>
+    <t xml:space="preserve">ЗАЯВКА №  / Дата 04.05.2016</t>
   </si>
   <si>
     <t>7.1 МИКРОБИОЛОГИЧНО ИЗПИТВАНЕ</t>
@@ -49,13 +49,43 @@
     <t>Забележка</t>
   </si>
   <si>
-    <t>Срок за изпитване: #D дни</t>
+    <t>1. p1</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>3234</t>
+  </si>
+  <si>
+    <t>МКБ</t>
+  </si>
+  <si>
+    <t>2. p2</t>
+  </si>
+  <si>
+    <t>E. Coli</t>
+  </si>
+  <si>
+    <t>ISO 16649-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Срок за изпитване:  дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>
   </si>
   <si>
     <t>7.2 ФИЗИКОХИМИЧНО И ОРГАНОЛЕПТИЧНО ИЗПИТВАНЕ</t>
+  </si>
+  <si>
+    <t>Бацилус</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> БДС ...</t>
+  </si>
+  <si>
+    <t>ФЗХ</t>
   </si>
 </sst>
 </file>
@@ -425,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -531,88 +561,130 @@
       <c r="A10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>12</v>
+      <c r="C20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -620,11 +692,11 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Requests should be completed
</commit_message>
<xml_diff>
--- a/Files/50000-51000/50278/50278_RequestList.xlsx
+++ b/Files/50000-51000/50278/50278_RequestList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">ФК 404-4   </t>
   </si>
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">ЗАЯВКА №  / Дата 04.05.2016</t>
+    <t>ЗАЯВКА № A/B50278 / Дата 07.05.2016</t>
   </si>
   <si>
     <t>7.1 МИКРОБИОЛОГИЧНО ИЗПИТВАНЕ</t>
@@ -34,7 +34,7 @@
     <t>Вх. №</t>
   </si>
   <si>
-    <t xml:space="preserve">Вид на  пробата</t>
+    <t>Вид на пробата</t>
   </si>
   <si>
     <t>Показател</t>
@@ -49,6 +49,9 @@
     <t>Забележка</t>
   </si>
   <si>
+    <t>A/B50278</t>
+  </si>
+  <si>
     <t>1. p1</t>
   </si>
   <si>
@@ -58,9 +61,6 @@
     <t>3234</t>
   </si>
   <si>
-    <t>МКБ</t>
-  </si>
-  <si>
     <t>2. p2</t>
   </si>
   <si>
@@ -70,7 +70,7 @@
     <t>ISO 16649-2</t>
   </si>
   <si>
-    <t xml:space="preserve">Срок за изпитване:  дни</t>
+    <t>Срок за изпитване: 11 дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve"> БДС ...</t>
-  </si>
-  <si>
-    <t>ФЗХ</t>
   </si>
 </sst>
 </file>
@@ -93,7 +90,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +105,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,11 +135,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -141,7 +166,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -150,6 +174,24 @@
     </xf>
     <xf fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment indent="2"/>
+    </xf>
+    <xf fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,34 +520,34 @@
       <c r="G1" s="4"/>
     </row>
     <row r="3" ht="18.75">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" ht="18.75">
       <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -525,71 +567,70 @@
       </c>
     </row>
     <row r="7" ht="18.75">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5"/>
+      <c r="A10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11">
-      <c r="B11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="0" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -598,7 +639,7 @@
       <c r="C13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
@@ -609,7 +650,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -629,46 +670,48 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20">
-      <c r="B20" s="0" t="s">
+    <row r="19">
+      <c r="A19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="B19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -677,7 +720,7 @@
       <c r="C21" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="0" t="s">

</xml_diff>